<commit_message>
Swapped x and y in 'data matrices' file
</commit_message>
<xml_diff>
--- a/FBG_Needle_Calibration_Data/needle_1/Jig_Calibration/Data Matrices.xlsx
+++ b/FBG_Needle_Calibration_Data/needle_1/Jig_Calibration/Data Matrices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epyan\Documents\JHU\Research\Shape Sensing\FBG_Needle_Calibration_Data\needle_1\Jig_Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16F9E07-3FF4-4603-A35D-0C5F1CD39B4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9BB5E0-7009-438A-A5FA-177EC92DC7CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12960" yWindow="60" windowWidth="10032" windowHeight="12024" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AA1" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -400,42 +402,42 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="B5">
-        <v>1.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="B6">
-        <v>1.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="B8">
-        <v>2.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -448,42 +450,42 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
         <v>0.8</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
         <v>1.25</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
         <v>1.6</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
         <v>2</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14">
         <v>2.5</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Reran jig calibration matrices again... still looks suspect
</commit_message>
<xml_diff>
--- a/FBG_Needle_Calibration_Data/needle_1/Jig_Calibration/Data Matrices.xlsx
+++ b/FBG_Needle_Calibration_Data/needle_1/Jig_Calibration/Data Matrices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epyan\Documents\JHU\Research\Shape Sensing\FBG_Needle_Calibration_Data\needle_1\Jig_Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9BB5E0-7009-438A-A5FA-177EC92DC7CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F67D00-3F04-4416-81EB-EEFC38C2C589}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9312" yWindow="120" windowWidth="13368" windowHeight="12096" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AA1" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:B14"/>
     </sheetView>
   </sheetViews>
@@ -402,7 +402,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0.8</v>
+        <v>-9.0395480225988699E-5</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -410,7 +410,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>1.25</v>
+        <v>-1.4124293785310735E-4</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -418,7 +418,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1.6</v>
+        <v>-1.807909604519774E-4</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -426,7 +426,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2</v>
+        <v>-2.2598870056497175E-4</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -434,7 +434,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2.5</v>
+        <v>-2.824858757062147E-4</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -453,7 +453,7 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <v>0.8</v>
+        <v>-9.0395480225988699E-5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -461,7 +461,7 @@
         <v>0</v>
       </c>
       <c r="B11">
-        <v>1.25</v>
+        <v>-1.4124293785310735E-4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -469,7 +469,7 @@
         <v>0</v>
       </c>
       <c r="B12">
-        <v>1.6</v>
+        <v>-1.807909604519774E-4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -477,7 +477,7 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>-2.2598870056497175E-4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -485,7 +485,7 @@
         <v>0</v>
       </c>
       <c r="B14">
-        <v>2.5</v>
+        <v>-2.824858757062147E-4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74764C02-81CB-4A9C-ACBE-6DE8EE6F6126}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:C29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,42 +674,42 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0</v>
+        <v>-9.0395480225988699E-5</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0</v>
+        <v>-1.4124293785310735E-4</v>
       </c>
       <c r="B5">
-        <v>1.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0</v>
+        <v>-1.807909604519774E-4</v>
       </c>
       <c r="B6">
-        <v>1.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0</v>
+        <v>-2.2598870056497175E-4</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0</v>
+        <v>-2.824858757062147E-4</v>
       </c>
       <c r="B8">
-        <v>2.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -722,42 +722,42 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>-9.0395480225988699E-5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>-1.4124293785310735E-4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>-1.807909604519774E-4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>-2.2598870056497175E-4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>-2.824858757062147E-4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -918,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4487B25B-71B3-4C38-BECD-AA929ED31E69}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,42 +947,42 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>0</v>
+        <v>-9.0395480225988699E-5</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0</v>
+        <v>-1.4124293785310735E-4</v>
       </c>
       <c r="B5">
-        <v>1.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0</v>
+        <v>-1.807909604519774E-4</v>
       </c>
       <c r="B6">
-        <v>1.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0</v>
+        <v>-2.2598870056497175E-4</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0</v>
+        <v>-2.824858757062147E-4</v>
       </c>
       <c r="B8">
-        <v>2.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -995,42 +995,42 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>-9.0395480225988699E-5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>-1.4124293785310735E-4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>-1.807909604519774E-4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>-2.2598870056497175E-4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>-2.824858757062147E-4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>